<commit_message>
MFY auto commit at 01/12/2021 14:06:58
</commit_message>
<xml_diff>
--- a/AdmitCard/MidDateSheet.xlsx
+++ b/AdmitCard/MidDateSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="825" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1545" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>CG-C3</t>
   </si>
@@ -86,6 +86,21 @@
   </si>
   <si>
     <t>Principles of Management</t>
+  </si>
+  <si>
+    <t>Tuesday, 30 Nov 11:30 to 1:00</t>
+  </si>
+  <si>
+    <t>Firday, 3 Dec 9:30 to 11:00</t>
+  </si>
+  <si>
+    <t>Wednesday, 1 Dec 11:30 to 1:00</t>
+  </si>
+  <si>
+    <t>Saturday, 4 Dec 9:30 to 11:00</t>
+  </si>
+  <si>
+    <t>Sunday, 30 Dec 2:00 to 3:30</t>
   </si>
 </sst>
 </file>
@@ -433,198 +448,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F16"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A3:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="36" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="37.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="36" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="2" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="2" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="2" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="2" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
+  <mergeCells count="24">
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="B15:B16"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="D3:D16"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="E3:E10"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="D3:D16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="77" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>